<commit_message>
Major change. Pushing out UiPath API, UiPathScaffold API, Enhanced-REFramework_Generator
</commit_message>
<xml_diff>
--- a/SequencesToScaffold.xlsx
+++ b/SequencesToScaffold.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrbla11\Documents\Programming\UiPathScaffolding\UiPath-Scaffold\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrbla11\Documents\Programming\UiPathScaffolding\UiPath-Scaffold-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE697EC-E0D5-47D0-92D3-C6BA8AC078E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD52FA8-C0E7-4A7C-BF24-F20EB79852F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4B821D92-83B0-43E6-87FF-FD8981F3A855}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>NAME</t>
   </si>
@@ -42,46 +42,7 @@
     <t>PARENT</t>
   </si>
   <si>
-    <t>Get Collection From Excel</t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t>OracleEBS Log Out</t>
-  </si>
-  <si>
-    <t>OracleEBS Expand NavItem</t>
-  </si>
-  <si>
-    <t>OracleEBS/</t>
-  </si>
-  <si>
-    <t>Excel/</t>
-  </si>
-  <si>
-    <t>OracleEBS NavigateTo Item</t>
-  </si>
-  <si>
-    <t>OracleEBS Recursive FindNavItem</t>
-  </si>
-  <si>
     <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Gets a collection from an excel document.</t>
-  </si>
-  <si>
-    <t>Logs out of Oracle EBS. Precondition: Oracle is open and logged in.</t>
-  </si>
-  <si>
-    <t>Expands a NavItem in Oracle EBS. Precondition: Oracle must be open and logged in.</t>
-  </si>
-  <si>
-    <t>Navigates to an item in Oracle EBS. Precondition: Oracle must be open and logged in.</t>
-  </si>
-  <si>
-    <t>Recursive function used to find a nav item in Oracle EBS. Must be called by OracleEBS NavigateTo Item.</t>
   </si>
 </sst>
 </file>
@@ -442,9 +403,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F49AF27D-FA31-4743-8DA0-A0A6E7DAC302}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -465,77 +428,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>